<commit_message>
added repr methods for df pretty pring, SelectableDataFrame class for selct() method persistance
</commit_message>
<xml_diff>
--- a/tests/test_project_data/raw_data.xlsx
+++ b/tests/test_project_data/raw_data.xlsx
@@ -494,9 +494,7 @@
       <c r="F2" t="n">
         <v>-0.3037714512320482</v>
       </c>
-      <c r="G2" t="n">
-        <v>-0.157988909446189</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>1.258191396404583</v>
       </c>
@@ -520,9 +518,7 @@
       <c r="F3" t="n">
         <v>-0.7787399985940539</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.6774322710687918</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>1.312343494363936</v>
       </c>
@@ -546,9 +542,7 @@
       <c r="F4" t="n">
         <v>0.8670539083516856</v>
       </c>
-      <c r="G4" t="n">
-        <v>-0.3419631957862002</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>-0.440453157735961</v>
       </c>
@@ -572,9 +566,7 @@
       <c r="F5" t="n">
         <v>1.1217632613896</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.3119044964081157</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>-0.5328676206298573</v>
       </c>
@@ -598,9 +590,7 @@
       <c r="F6" t="n">
         <v>1.364495219432429</v>
       </c>
-      <c r="G6" t="n">
-        <v>1.054415203637279</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>-0.05451619123091781</v>
       </c>
@@ -624,9 +614,7 @@
       <c r="F7" t="n">
         <v>0.4368111890008604</v>
       </c>
-      <c r="G7" t="n">
-        <v>0.2601101889178086</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>-0.819502599620287</v>
       </c>
@@ -650,9 +638,7 @@
       <c r="F8" t="n">
         <v>-0.09451595297682103</v>
       </c>
-      <c r="G8" t="n">
-        <v>-1.04685227871025</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>-1.212319162941807</v>
       </c>
@@ -676,9 +662,7 @@
       <c r="F9" t="n">
         <v>-1.674522900941328</v>
       </c>
-      <c r="G9" t="n">
-        <v>-0.1839786443002082</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>-0.2841891267935588</v>
       </c>
@@ -702,9 +686,7 @@
       <c r="F10" t="n">
         <v>-0.1528875008420571</v>
       </c>
-      <c r="G10" t="n">
-        <v>-0.4264706832516852</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>-0.8471137186165356</v>
       </c>
@@ -728,9 +710,7 @@
       <c r="F11" t="n">
         <v>-0.5223194224941036</v>
       </c>
-      <c r="G11" t="n">
-        <v>2.150618545057953</v>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
         <v>0.2492105324991214</v>
       </c>
@@ -754,9 +734,7 @@
       <c r="F12" t="n">
         <v>-0.6112098346586816</v>
       </c>
-      <c r="G12" t="n">
-        <v>-1.913804561114032</v>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
         <v>0.3832090099613838</v>
       </c>
@@ -778,9 +756,7 @@
       <c r="F13" t="n">
         <v>-1.225209928769799</v>
       </c>
-      <c r="G13" t="n">
-        <v>1.186487895223491</v>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>1.076991788866259</v>
       </c>
@@ -804,9 +780,7 @@
       <c r="F14" t="n">
         <v>0.09989159755581106</v>
       </c>
-      <c r="G14" t="n">
-        <v>1.922073797490591</v>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>0.2494804630131531</v>
       </c>
@@ -830,9 +804,7 @@
       <c r="F15" t="n">
         <v>2.371785148507819</v>
       </c>
-      <c r="G15" t="n">
-        <v>-1.894568765630599</v>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>-1.443609141727901</v>
       </c>
@@ -856,9 +828,7 @@
       <c r="F16" t="n">
         <v>0.18276113175439</v>
       </c>
-      <c r="G16" t="n">
-        <v>-0.3575620154905805</v>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>-0.04625462971449715</v>
       </c>
@@ -882,9 +852,7 @@
       <c r="F17" t="n">
         <v>0.07401424352142075</v>
       </c>
-      <c r="G17" t="n">
-        <v>0.6665189843481726</v>
-      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
         <v>-1.851697065097567</v>
       </c>
@@ -908,9 +876,7 @@
       <c r="F18" t="n">
         <v>-0.2857010560763674</v>
       </c>
-      <c r="G18" t="n">
-        <v>0.06049788381686377</v>
-      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>-0.2123062595485593</v>
       </c>
@@ -932,9 +898,7 @@
       <c r="F19" t="n">
         <v>-0.2845790951334837</v>
       </c>
-      <c r="G19" t="n">
-        <v>-0.1460660619208632</v>
-      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
         <v>0.4232519291396334</v>
       </c>
@@ -958,9 +922,7 @@
       <c r="F20" t="n">
         <v>-0.1789597588930808</v>
       </c>
-      <c r="G20" t="n">
-        <v>0.9966364148975468</v>
-      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
         <v>1.12635330327993</v>
       </c>
@@ -984,9 +946,7 @@
       <c r="F21" t="n">
         <v>0.7749248052157985</v>
       </c>
-      <c r="G21" t="n">
-        <v>-0.3381351584863113</v>
-      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>-1.112004795155405</v>
       </c>
@@ -1010,9 +970,7 @@
       <c r="F22" t="n">
         <v>-0.5783595434725717</v>
       </c>
-      <c r="G22" t="n">
-        <v>-1.602876821805252</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>0.2534244611323342</v>
       </c>
@@ -1036,9 +994,7 @@
       <c r="F23" t="n">
         <v>0.3182750993405906</v>
       </c>
-      <c r="G23" t="n">
-        <v>-2.10749749939844</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>-2.095967051686733</v>
       </c>
@@ -1062,9 +1018,7 @@
       <c r="F24" t="n">
         <v>0.3067392146007051</v>
       </c>
-      <c r="G24" t="n">
-        <v>1.546614813934637</v>
-      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
         <v>1.72614781587838</v>
       </c>
@@ -1088,9 +1042,7 @@
       <c r="F25" t="n">
         <v>-1.810626101138616</v>
       </c>
-      <c r="G25" t="n">
-        <v>0.3511526509428524</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>-1.940864132969403</v>
       </c>
@@ -1114,9 +1066,7 @@
       <c r="F26" t="n">
         <v>0.2356647775751688</v>
       </c>
-      <c r="G26" t="n">
-        <v>0.706578282543686</v>
-      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
         <v>0.6346988222299508</v>
       </c>
@@ -1140,9 +1090,7 @@
       <c r="F27" t="n">
         <v>0.8664267598066455</v>
       </c>
-      <c r="G27" t="n">
-        <v>0.02427275316091584</v>
-      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
         <v>0.4588695265057765</v>
       </c>
@@ -1166,9 +1114,7 @@
       <c r="F28" t="n">
         <v>0.09011813172283145</v>
       </c>
-      <c r="G28" t="n">
-        <v>-0.06327105646139243</v>
-      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
         <v>-0.1799400384753524</v>
       </c>
@@ -1192,9 +1138,7 @@
       <c r="F29" t="n">
         <v>1.32723524836545</v>
       </c>
-      <c r="G29" t="n">
-        <v>-1.284811717814379</v>
-      </c>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
         <v>-0.9604329109277333</v>
       </c>
@@ -1218,9 +1162,7 @@
       <c r="F30" t="n">
         <v>1.381434342422084</v>
       </c>
-      <c r="G30" t="n">
-        <v>0.0285943954112818</v>
-      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
         <v>0.3495284451194932</v>
       </c>
@@ -1244,9 +1186,7 @@
       <c r="F31" t="n">
         <v>1.735763817053581</v>
       </c>
-      <c r="G31" t="n">
-        <v>0.2341817973095726</v>
-      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
         <v>-0.01373019559161995</v>
       </c>
@@ -1270,9 +1210,7 @@
       <c r="F32" t="n">
         <v>-0.08270747252074159</v>
       </c>
-      <c r="G32" t="n">
-        <v>0.7538849996361171</v>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
         <v>1.102061436041613</v>
       </c>
@@ -1296,9 +1234,7 @@
       <c r="F33" t="n">
         <v>-0.2473674654935561</v>
       </c>
-      <c r="G33" t="n">
-        <v>1.298128159837914</v>
-      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
         <v>0.7119734431346667</v>
       </c>
@@ -1322,9 +1258,7 @@
       <c r="F34" t="n">
         <v>-0.3616127346563344</v>
       </c>
-      <c r="G34" t="n">
-        <v>-0.932764939221977</v>
-      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
         <v>0.3388528846911539</v>
       </c>
@@ -1348,9 +1282,7 @@
       <c r="F35" t="n">
         <v>0.9327942870960271</v>
       </c>
-      <c r="G35" t="n">
-        <v>0.8886572089665434</v>
-      </c>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
         <v>-1.575514652084737</v>
       </c>
@@ -1374,9 +1306,7 @@
       <c r="F36" t="n">
         <v>0.782967685321958</v>
       </c>
-      <c r="G36" t="n">
-        <v>-0.7745009492613354</v>
-      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
         <v>0.7038623380135581</v>
       </c>
@@ -1400,9 +1330,7 @@
       <c r="F37" t="n">
         <v>-1.002452249154467</v>
       </c>
-      <c r="G37" t="n">
-        <v>-0.02207876711224952</v>
-      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
         <v>-1.557126049667482</v>
       </c>
@@ -1426,9 +1354,7 @@
       <c r="F38" t="n">
         <v>1.022941202303604</v>
       </c>
-      <c r="G38" t="n">
-        <v>-1.174117488690212</v>
-      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
         <v>1.174868850184188</v>
       </c>
@@ -1452,9 +1378,7 @@
       <c r="F39" t="n">
         <v>1.044513622800114</v>
       </c>
-      <c r="G39" t="n">
-        <v>1.669418187304373</v>
-      </c>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
         <v>-0.3394886821652572</v>
       </c>
@@ -1478,9 +1402,7 @@
       <c r="F40" t="n">
         <v>0.127881379821939</v>
       </c>
-      <c r="G40" t="n">
-        <v>-0.8419745661900426</v>
-      </c>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
         <v>1.19955969653429</v>
       </c>
@@ -1504,9 +1426,7 @@
       <c r="F41" t="n">
         <v>-1.945075494766041</v>
       </c>
-      <c r="G41" t="n">
-        <v>0.3455956536378763</v>
-      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
         <v>1.715724431757643</v>
       </c>
@@ -1530,9 +1450,7 @@
       <c r="F42" t="n">
         <v>1.904496731705125</v>
       </c>
-      <c r="G42" t="n">
-        <v>0.7480180626701455</v>
-      </c>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
         <v>-1.83667860511828</v>
       </c>
@@ -1556,9 +1474,7 @@
       <c r="F43" t="n">
         <v>0.4476656872031483</v>
       </c>
-      <c r="G43" t="n">
-        <v>-1.021031322402895</v>
-      </c>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
         <v>0.3532862779121294</v>
       </c>
@@ -1582,9 +1498,7 @@
       <c r="F44" t="n">
         <v>1.659986153352299</v>
       </c>
-      <c r="G44" t="n">
-        <v>-1.078361904554094</v>
-      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
         <v>-0.6021757054938222</v>
       </c>
@@ -1608,9 +1522,7 @@
       <c r="F45" t="n">
         <v>0.345972903213777</v>
       </c>
-      <c r="G45" t="n">
-        <v>-2.428400303884889</v>
-      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
         <v>0.3672949061525647</v>
       </c>
@@ -1632,9 +1544,7 @@
       <c r="F46" t="n">
         <v>0.7469395384586477</v>
       </c>
-      <c r="G46" t="n">
-        <v>0.5771009354687265</v>
-      </c>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
         <v>-2.56562305804699</v>
       </c>
@@ -1658,9 +1568,7 @@
       <c r="F47" t="n">
         <v>0.03898644860885329</v>
       </c>
-      <c r="G47" t="n">
-        <v>-0.116149119248953</v>
-      </c>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
         <v>-1.286328277286238</v>
       </c>
@@ -1684,9 +1592,7 @@
       <c r="F48" t="n">
         <v>1.574096561016636</v>
       </c>
-      <c r="G48" t="n">
-        <v>1.39554604516858</v>
-      </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
         <v>-0.4643721814536547</v>
       </c>
@@ -1710,9 +1616,7 @@
       <c r="F49" t="n">
         <v>-0.2855585751778168</v>
       </c>
-      <c r="G49" t="n">
-        <v>-2.004826739554117</v>
-      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
         <v>-0.5275015283724449</v>
       </c>
@@ -1736,9 +1640,7 @@
       <c r="F50" t="n">
         <v>0.1447676700118066</v>
       </c>
-      <c r="G50" t="n">
-        <v>0.4352439391925884</v>
-      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
         <v>2.998385639998854</v>
       </c>
@@ -1762,9 +1664,7 @@
       <c r="F51" t="n">
         <v>-0.520621957260065</v>
       </c>
-      <c r="G51" t="n">
-        <v>0.6979684595151631</v>
-      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
         <v>0.5206696981906984</v>
       </c>
@@ -1788,9 +1688,7 @@
       <c r="F52" t="n">
         <v>-0.795495273740608</v>
       </c>
-      <c r="G52" t="n">
-        <v>0.7824057657358687</v>
-      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
         <v>0.02940928694209497</v>
       </c>
@@ -1814,9 +1712,7 @@
       <c r="F53" t="n">
         <v>-0.1823683686102011</v>
       </c>
-      <c r="G53" t="n">
-        <v>0.2584098266617079</v>
-      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
         <v>2.145228762377485</v>
       </c>
@@ -1840,9 +1736,7 @@
       <c r="F54" t="n">
         <v>-1.150564355426252</v>
       </c>
-      <c r="G54" t="n">
-        <v>1.626882468845689</v>
-      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
         <v>-0.04928349316358954</v>
       </c>
@@ -1866,9 +1760,7 @@
       <c r="F55" t="n">
         <v>0.3185126992607578</v>
       </c>
-      <c r="G55" t="n">
-        <v>-0.4180540682490512</v>
-      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
         <v>-0.08828919560650457</v>
       </c>
@@ -1892,9 +1784,7 @@
       <c r="F56" t="n">
         <v>-2.771565991674202</v>
       </c>
-      <c r="G56" t="n">
-        <v>-1.488063264778056</v>
-      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
         <v>-0.2410880821202202</v>
       </c>
@@ -1918,9 +1808,7 @@
       <c r="F57" t="n">
         <v>0.3494149065911288</v>
       </c>
-      <c r="G57" t="n">
-        <v>-0.2962866635456528</v>
-      </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
         <v>-0.4000639931184808</v>
       </c>
@@ -1944,9 +1832,7 @@
       <c r="F58" t="n">
         <v>-0.8435291635675959</v>
       </c>
-      <c r="G58" t="n">
-        <v>-0.1257235525306267</v>
-      </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
         <v>0.6725902375889932</v>
       </c>
@@ -1970,9 +1856,7 @@
       <c r="F59" t="n">
         <v>0.7048867971501362</v>
       </c>
-      <c r="G59" t="n">
-        <v>0.1139850919808841</v>
-      </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
         <v>0.4484303279396845</v>
       </c>
@@ -1996,9 +1880,7 @@
       <c r="F60" t="n">
         <v>0.1259980593958571</v>
       </c>
-      <c r="G60" t="n">
-        <v>-0.7608966322770548</v>
-      </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
         <v>-0.02546178409508416</v>
       </c>
@@ -2022,9 +1904,7 @@
       <c r="F61" t="n">
         <v>0.5417437454977816</v>
       </c>
-      <c r="G61" t="n">
-        <v>0.1720435233429299</v>
-      </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
         <v>0.3687084117029405</v>
       </c>
@@ -2048,9 +1928,7 @@
       <c r="F62" t="n">
         <v>-1.490590336870925</v>
       </c>
-      <c r="G62" t="n">
-        <v>-2.028776703243214</v>
-      </c>
+      <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
         <v>0.704761980519689</v>
       </c>
@@ -2074,9 +1952,7 @@
       <c r="F63" t="n">
         <v>-0.8085990251483246</v>
       </c>
-      <c r="G63" t="n">
-        <v>0.1544612710722488</v>
-      </c>
+      <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
         <v>-0.4230802561772284</v>
       </c>
@@ -2100,9 +1976,7 @@
       <c r="F64" t="n">
         <v>-0.5858157745164355</v>
       </c>
-      <c r="G64" t="n">
-        <v>0.7516166860403254</v>
-      </c>
+      <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
         <v>-0.1243402768678577</v>
       </c>
@@ -2126,9 +2000,7 @@
       <c r="F65" t="n">
         <v>-0.8203465676437375</v>
       </c>
-      <c r="G65" t="n">
-        <v>-0.2957100276834215</v>
-      </c>
+      <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
         <v>0.5679678230631531</v>
       </c>

</xml_diff>